<commit_message>
fix: se solucionar errores
</commit_message>
<xml_diff>
--- a/documents/empresas.xlsx
+++ b/documents/empresas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -896,10 +896,8 @@
           <t>razon social de prueba</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>8894</t>
-        </is>
+      <c r="C14" t="n">
+        <v>8894</v>
       </c>
       <c r="D14" t="n">
         <v>1073</v>
@@ -922,6 +920,44 @@
       <c r="H14" t="inlineStr">
         <is>
           <t>123212</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>razon social 1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>12545</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>4330</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Terminación y acabado de edificios</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>representante 1</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>correo 1</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>telefono 1</t>
         </is>
       </c>
     </row>

</xml_diff>